<commit_message>
Update Go code to skip first 10 rows in CSV files
- Modified readCSVFile function to skip first 10 rows and start reading from row 11
- Added proper error handling for files with fewer than 10 rows
- Enhanced user feedback to indicate row skipping behavior
- Updated main function with better status messages and error handling
- Added test CSV files with realistic NetSuite header structure
- Maintains data integrity while handling NetSuite export format
- Improved processing feedback showing actual data rows processed

This addresses the NetSuite CSV format where data starts at row 11.

Co-authored-by: ddecoen <85462083+ddecoen@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/coder_financial_package.xlsx
+++ b/coder_financial_package.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
   <si>
     <t>Financial Row</t>
   </si>
@@ -63,6 +63,36 @@
     <t>-6.38%</t>
   </si>
   <si>
+    <t>Prepaid expenses</t>
+  </si>
+  <si>
+    <t>$1,396,603.84</t>
+  </si>
+  <si>
+    <t>$1,436,064.00</t>
+  </si>
+  <si>
+    <t>($39,460.16)</t>
+  </si>
+  <si>
+    <t>-2.75%</t>
+  </si>
+  <si>
+    <t>Total Current Assets</t>
+  </si>
+  <si>
+    <t>$28,086,600.03</t>
+  </si>
+  <si>
+    <t>$29,493,770.49</t>
+  </si>
+  <si>
+    <t>($1,407,170.46)</t>
+  </si>
+  <si>
+    <t>-4.77%</t>
+  </si>
+  <si>
     <t>Total Assets</t>
   </si>
   <si>
@@ -78,6 +108,51 @@
     <t>-4.68%</t>
   </si>
   <si>
+    <t>Accounts Payable</t>
+  </si>
+  <si>
+    <t>$588,450.01</t>
+  </si>
+  <si>
+    <t>$333,741.90</t>
+  </si>
+  <si>
+    <t>$254,708.11</t>
+  </si>
+  <si>
+    <t>76.32%</t>
+  </si>
+  <si>
+    <t>Deferred revenue</t>
+  </si>
+  <si>
+    <t>$2,343,160.23</t>
+  </si>
+  <si>
+    <t>$2,281,494.61</t>
+  </si>
+  <si>
+    <t>$61,665.62</t>
+  </si>
+  <si>
+    <t>2.70%</t>
+  </si>
+  <si>
+    <t>Total Equity</t>
+  </si>
+  <si>
+    <t>$24,403,574.05</t>
+  </si>
+  <si>
+    <t>$26,254,039.93</t>
+  </si>
+  <si>
+    <t>($1,850,465.88)</t>
+  </si>
+  <si>
+    <t>-7.05%</t>
+  </si>
+  <si>
     <t>Amount (Jun 2025)</t>
   </si>
   <si>
@@ -127,6 +202,51 @@
   </si>
   <si>
     <t>6.49%</t>
+  </si>
+  <si>
+    <t>Gross Profit</t>
+  </si>
+  <si>
+    <t>$1,223,682.10</t>
+  </si>
+  <si>
+    <t>$1,145,606.48</t>
+  </si>
+  <si>
+    <t>$78,075.62</t>
+  </si>
+  <si>
+    <t>6.82%</t>
+  </si>
+  <si>
+    <t>Salaries</t>
+  </si>
+  <si>
+    <t>$1,380,987.81</t>
+  </si>
+  <si>
+    <t>$1,326,380.04</t>
+  </si>
+  <si>
+    <t>$54,607.77</t>
+  </si>
+  <si>
+    <t>4.12%</t>
+  </si>
+  <si>
+    <t>Total Operating expenses</t>
+  </si>
+  <si>
+    <t>$3,224,657.83</t>
+  </si>
+  <si>
+    <t>$2,919,932.52</t>
+  </si>
+  <si>
+    <t>$304,725.31</t>
+  </si>
+  <si>
+    <t>10.44%</t>
   </si>
   <si>
     <t>Net Income</t>
@@ -529,6 +649,91 @@
         <v>19</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
@@ -545,10 +750,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -559,70 +764,121 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>